<commit_message>
Modificar plantilla y ejemplo diccionario
</commit_message>
<xml_diff>
--- a/assets/excel/plantilla_diccionario.xlsx
+++ b/assets/excel/plantilla_diccionario.xlsx
@@ -12,62 +12,100 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="32">
-  <si>
-    <r>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="30">
+  <si>
+    <r>
+      <rPr>
+        <rFont val="Muli, Arial"/>
+        <b/>
+        <color rgb="FF000000"/>
+        <sz val="9.0"/>
+      </rPr>
       <t xml:space="preserve">Nombre de la base y/o conjunto de datos
 </t>
     </r>
     <r>
       <rPr>
+        <rFont val="Muli, Arial"/>
+        <b val="0"/>
+        <color rgb="FF000000"/>
         <sz val="8.0"/>
       </rPr>
       <t>(Repetir el nombre en todas las filas</t>
     </r>
     <r>
-      <rPr/>
+      <rPr>
+        <rFont val="Muli, Arial"/>
+        <b val="0"/>
+        <color rgb="FF000000"/>
+        <sz val="9.0"/>
+      </rPr>
       <t>)</t>
     </r>
   </si>
   <si>
     <r>
+      <rPr>
+        <rFont val="Muli, Arial"/>
+        <b/>
+        <color theme="1"/>
+        <sz val="9.0"/>
+      </rPr>
       <t xml:space="preserve">Nombre de la tabla de la base de datos / hoja del conjunto de datos
 </t>
     </r>
     <r>
       <rPr>
+        <rFont val="Muli, Arial"/>
+        <b val="0"/>
+        <color theme="1"/>
         <sz val="8.0"/>
       </rPr>
       <t xml:space="preserve">(En caso de que no existan numerosas tablas u hojas escribir </t>
     </r>
     <r>
       <rPr>
+        <rFont val="Muli, Arial"/>
+        <b val="0"/>
         <i/>
+        <color theme="1"/>
         <sz val="8.0"/>
       </rPr>
       <t>“No aplica"</t>
     </r>
     <r>
       <rPr>
+        <rFont val="Muli, Arial"/>
+        <b val="0"/>
+        <color theme="1"/>
         <sz val="8.0"/>
       </rPr>
       <t>)</t>
     </r>
   </si>
   <si>
-    <t>Etiqueta</t>
+    <t>Etiqueta del campo o variable (atributo)</t>
   </si>
   <si>
     <t>Descripción</t>
   </si>
   <si>
     <r>
-      <t xml:space="preserve">Tipo de variable,  campo o atributo
+      <rPr>
+        <rFont val="Muli, Arial"/>
+        <b/>
+        <color theme="1"/>
+        <sz val="9.0"/>
+      </rPr>
+      <t xml:space="preserve">Tipo de dato
 </t>
     </r>
     <r>
       <rPr>
+        <rFont val="Muli, Arial"/>
+        <b val="0"/>
         <i/>
+        <color theme="1"/>
         <sz val="8.0"/>
       </rPr>
       <t>(Seleccione de acuerdo a las opciones)</t>
@@ -79,42 +117,72 @@
   </si>
   <si>
     <r>
+      <rPr>
+        <rFont val="Muli, Arial"/>
+        <b/>
+        <color theme="1"/>
+        <sz val="9.0"/>
+      </rPr>
       <t xml:space="preserve">Clasificación de la información
 </t>
     </r>
     <r>
       <rPr>
+        <rFont val="Muli, Arial"/>
+        <b val="0"/>
+        <color theme="1"/>
         <sz val="8.0"/>
       </rPr>
       <t xml:space="preserve">
 </t>
     </r>
     <r>
-      <rPr/>
+      <rPr>
+        <rFont val="Muli, Arial"/>
+        <b val="0"/>
+        <color theme="1"/>
+        <sz val="9.0"/>
+      </rPr>
       <t xml:space="preserve">
 </t>
     </r>
     <r>
       <rPr>
+        <rFont val="Muli, Arial"/>
+        <b val="0"/>
         <i/>
+        <color theme="1"/>
         <sz val="8.0"/>
       </rPr>
       <t>(Seleccione de acuerdo a las opciones</t>
     </r>
     <r>
       <rPr>
+        <rFont val="Muli, Arial"/>
+        <b val="0"/>
         <i/>
+        <color theme="1"/>
+        <sz val="9.0"/>
       </rPr>
       <t>)</t>
     </r>
   </si>
   <si>
     <r>
+      <rPr>
+        <rFont val="Muli, Arial"/>
+        <b/>
+        <color theme="1"/>
+        <sz val="9.0"/>
+      </rPr>
       <t xml:space="preserve">Especificaciones y/o reglas de cálculo
 </t>
     </r>
     <r>
       <rPr>
+        <rFont val="Muli, Arial"/>
+        <b val="0"/>
+        <color theme="1"/>
         <sz val="8.0"/>
       </rPr>
       <t>(En caso de que este elemento no aplique a su base de datos y/o conjunto de datos, registre “No Aplica”)</t>
@@ -122,30 +190,67 @@
   </si>
   <si>
     <r>
+      <rPr>
+        <rFont val="Muli, Arial"/>
+        <b/>
+        <color theme="1"/>
+        <sz val="9.0"/>
+      </rPr>
       <t xml:space="preserve">Obligatoriedad del campo
 </t>
     </r>
     <r>
       <rPr>
+        <rFont val="Muli, Arial"/>
+        <b val="0"/>
+        <color theme="1"/>
         <sz val="8.0"/>
       </rPr>
       <t>(Seleccione de acuerdo a las opciones)</t>
     </r>
   </si>
   <si>
-    <t xml:space="preserve">Registro de campos vacíos 
+    <r>
+      <rPr>
+        <rFont val="Muli"/>
+        <b/>
+        <color theme="1"/>
+        <sz val="9.0"/>
+      </rPr>
+      <t xml:space="preserve">Registro de campos vacíos 
 </t>
+    </r>
+    <r>
+      <rPr>
+        <rFont val="Muli"/>
+        <b val="0"/>
+        <color theme="1"/>
+        <sz val="9.0"/>
+      </rPr>
+      <t>(Si este campo no tiene campos vacíos anotar "SIN DATOS VACÍOS")</t>
+    </r>
   </si>
   <si>
     <t>Tipo</t>
   </si>
   <si>
     <r>
+      <rPr>
+        <rFont val="Muli, Arial"/>
+        <b/>
+        <color theme="1"/>
+        <sz val="10.0"/>
+      </rPr>
       <t xml:space="preserve">Clasificación de la información
 </t>
     </r>
     <r>
-      <rPr/>
+      <rPr>
+        <rFont val="Muli, Arial"/>
+        <b val="0"/>
+        <color theme="1"/>
+        <sz val="10.0"/>
+      </rPr>
       <t>(reservada, confidencial, pública)</t>
     </r>
   </si>
@@ -156,7 +261,7 @@
     <t>Obligatoriedad del campo</t>
   </si>
   <si>
-    <t>Texto</t>
+    <t>Alfanumérico</t>
   </si>
   <si>
     <t>Reservada</t>
@@ -168,7 +273,7 @@
     <t xml:space="preserve">Obligatorio  </t>
   </si>
   <si>
-    <t>Alfanumérico</t>
+    <t>Número entero</t>
   </si>
   <si>
     <t>Confidencial</t>
@@ -180,15 +285,12 @@
     <t xml:space="preserve">Opcional </t>
   </si>
   <si>
-    <t>Número entero</t>
+    <t>Número con decimales</t>
   </si>
   <si>
     <t>Pública</t>
   </si>
   <si>
-    <t>Número con decimales</t>
-  </si>
-  <si>
     <t>Fecha</t>
   </si>
   <si>
@@ -205,9 +307,6 @@
   </si>
   <si>
     <t>Geometry</t>
-  </si>
-  <si>
-    <t>Proyección</t>
   </si>
 </sst>
 </file>
@@ -972,7 +1071,7 @@
   </conditionalFormatting>
   <dataValidations>
     <dataValidation type="list" allowBlank="1" sqref="E2:E25">
-      <formula1>Validadores!$A$2:$A$12</formula1>
+      <formula1>Validadores!$A$2:$A$10</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" sqref="G2:G25">
       <formula1>Validadores!$B$2:$B$4</formula1>
@@ -1098,22 +1197,6 @@
       <c r="C10" s="20"/>
       <c r="D10" s="20"/>
     </row>
-    <row r="11">
-      <c r="A11" s="19" t="s">
-        <v>30</v>
-      </c>
-      <c r="B11" s="20"/>
-      <c r="C11" s="20"/>
-      <c r="D11" s="20"/>
-    </row>
-    <row r="12">
-      <c r="A12" s="19" t="s">
-        <v>31</v>
-      </c>
-      <c r="B12" s="20"/>
-      <c r="C12" s="20"/>
-      <c r="D12" s="20"/>
-    </row>
   </sheetData>
   <drawing r:id="rId1"/>
 </worksheet>

</xml_diff>